<commit_message>
Update some datas and update the Slotstate() methods
</commit_message>
<xml_diff>
--- a/30_system_data/30-bus.xlsx
+++ b/30_system_data/30-bus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="branch data" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -336,6 +336,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -640,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -655,311 +657,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="D1" t="s">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>10</v>
+      <c r="D1">
+        <v>12.0198054991476</v>
+      </c>
+      <c r="E1" s="15">
+        <v>38.359448671118798</v>
+      </c>
+      <c r="F1" s="12">
+        <v>42.024453236031697</v>
+      </c>
+      <c r="G1" s="19">
+        <v>41.024453236031697</v>
+      </c>
+      <c r="H1" s="12">
+        <v>43.890868172438601</v>
+      </c>
+      <c r="I1" s="15">
+        <v>44.890868172438601</v>
+      </c>
+      <c r="J1" s="24">
+        <v>10000</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>12.0198054991476</v>
+        <v>15.627368075095999</v>
       </c>
       <c r="E2">
-        <v>38.359448671118798</v>
+        <v>30.103565135907601</v>
       </c>
       <c r="F2">
-        <v>42.024453236031697</v>
+        <v>35.867255012184899</v>
       </c>
       <c r="G2" s="9">
-        <v>41.024453236031697</v>
+        <v>37.167255012184903</v>
       </c>
       <c r="H2">
-        <v>43.890868172438601</v>
+        <v>35.158190864789603</v>
       </c>
       <c r="I2">
-        <v>44.890868172438601</v>
-      </c>
-      <c r="J2" s="2">
-        <v>10000</v>
+        <v>35.158190864789603</v>
+      </c>
+      <c r="J2" s="7">
+        <v>2.6833</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
-        <v>15.627368075095999</v>
+        <v>16.889755935606999</v>
       </c>
       <c r="E3">
-        <v>30.103565135907601</v>
+        <v>28.411850243896701</v>
       </c>
       <c r="F3">
-        <v>35.867255012184899</v>
+        <v>37.951560469010502</v>
       </c>
       <c r="G3" s="9">
-        <v>37.167255012184903</v>
+        <v>35.261560469010497</v>
       </c>
       <c r="H3">
-        <v>35.158190864789603</v>
+        <v>35.108777778523802</v>
       </c>
       <c r="I3">
-        <v>35.158190864789603</v>
-      </c>
-      <c r="J3" s="7">
-        <v>2.6833</v>
+        <v>35.108777778523802</v>
+      </c>
+      <c r="J3" s="8">
+        <v>43.890868172438601</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>16.889755935606999</v>
+        <v>14.509241513755899</v>
       </c>
       <c r="E4">
-        <v>28.411850243896701</v>
+        <v>19.616585698888699</v>
       </c>
       <c r="F4">
-        <v>37.951560469010502</v>
+        <v>22.928728374792001</v>
       </c>
       <c r="G4" s="9">
-        <v>35.261560469010497</v>
+        <v>24.928728374792001</v>
       </c>
       <c r="H4">
-        <v>35.108777778523802</v>
+        <v>21.489894238304199</v>
       </c>
       <c r="I4">
-        <v>35.108777778523802</v>
+        <v>31.711950779587099</v>
       </c>
       <c r="J4" s="8">
-        <v>43.890868172438601</v>
+        <v>35.158190864789603</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5">
-        <v>14.509241513755899</v>
+        <v>21.590745300686098</v>
       </c>
       <c r="E5">
-        <v>19.616585698888699</v>
+        <v>32.828421899276499</v>
       </c>
       <c r="F5">
-        <v>22.928728374792001</v>
+        <v>40.760838618257203</v>
       </c>
       <c r="G5" s="9">
-        <v>24.928728374792001</v>
+        <v>39.760838618257203</v>
       </c>
       <c r="H5">
+        <v>37.1533034709581</v>
+      </c>
+      <c r="I5">
         <v>21.489894238304199</v>
       </c>
-      <c r="I5">
-        <v>31.711950779587099</v>
-      </c>
       <c r="J5" s="8">
-        <v>35.158190864789603</v>
+        <v>35.108777778523802</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>21.590745300686098</v>
+        <v>13.2962299746242</v>
       </c>
       <c r="E6">
-        <v>32.828421899276499</v>
+        <v>27.082216862862001</v>
       </c>
       <c r="F6">
-        <v>40.760838618257203</v>
+        <v>32.310154700001597</v>
       </c>
       <c r="G6" s="9">
-        <v>39.760838618257203</v>
+        <v>28.469154700001599</v>
       </c>
       <c r="H6">
-        <v>37.1533034709581</v>
-      </c>
-      <c r="I6">
-        <v>21.489894238304199</v>
-      </c>
-      <c r="J6" s="8">
-        <v>35.108777778523802</v>
+        <v>31.711950779587099</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J6" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
       <c r="C7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>13.2962299746242</v>
+        <v>25.215564850458701</v>
       </c>
       <c r="E7">
-        <v>27.082216862862001</v>
+        <v>26.070994077773602</v>
       </c>
       <c r="F7">
-        <v>32.310154700001597</v>
+        <v>20.608733955612198</v>
       </c>
       <c r="G7" s="9">
-        <v>28.469154700001599</v>
+        <v>23.608733955612198</v>
       </c>
       <c r="H7">
+        <v>17.0996482487765</v>
+      </c>
+      <c r="I7">
+        <v>37.1533034709581</v>
+      </c>
+      <c r="J7" s="8">
         <v>31.711950779587099</v>
-      </c>
-      <c r="I7" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J7" s="2">
-        <v>10000</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D8">
-        <v>25.215564850458701</v>
+        <v>2.6238680204945299</v>
       </c>
       <c r="E8">
-        <v>26.070994077773602</v>
+        <v>21.245646262877699</v>
       </c>
       <c r="F8">
-        <v>20.608733955612198</v>
+        <v>41.348721023244899</v>
       </c>
       <c r="G8" s="9">
-        <v>23.608733955612198</v>
+        <v>39.348721023244899</v>
       </c>
       <c r="H8">
-        <v>17.0996482487765</v>
+        <v>41.058257494958397</v>
       </c>
       <c r="I8">
-        <v>37.1533034709581</v>
+        <v>0</v>
       </c>
       <c r="J8" s="8">
-        <v>31.711950779587099</v>
+        <v>21.850241129054901</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D9">
-        <v>2.6238680204945299</v>
+        <v>15.0263440702964</v>
       </c>
       <c r="E9">
-        <v>21.245646262877699</v>
+        <v>19.945890141241801</v>
       </c>
       <c r="F9">
-        <v>41.348721023244899</v>
+        <v>23.3081430694441</v>
       </c>
       <c r="G9" s="9">
-        <v>39.348721023244899</v>
+        <v>21.3081430694441</v>
       </c>
       <c r="H9">
-        <v>41.058257494958397</v>
+        <v>21.850241129054901</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>21.850241129054901</v>
+        <v>17.0996482487765</v>
+      </c>
+      <c r="J9" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>15.0263440702964</v>
+        <v>9.7961178272336493</v>
       </c>
       <c r="E10">
-        <v>19.945890141241801</v>
+        <v>5.0498306253105003</v>
       </c>
       <c r="F10">
-        <v>23.3081430694441</v>
+        <v>6.6347544528965701</v>
       </c>
       <c r="G10" s="9">
-        <v>21.3081430694441</v>
+        <v>8.6347544528965692</v>
       </c>
       <c r="H10">
+        <v>4.64960051236356</v>
+      </c>
+      <c r="I10">
         <v>21.850241129054901</v>
-      </c>
-      <c r="I10">
-        <v>17.0996482487765</v>
       </c>
       <c r="J10" s="2">
         <v>10000</v>
@@ -967,31 +978,31 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>6</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D11">
-        <v>9.7961178272336493</v>
+        <v>34.8264118509572</v>
       </c>
       <c r="E11">
-        <v>5.0498306253105003</v>
-      </c>
-      <c r="F11">
-        <v>6.6347544528965701</v>
-      </c>
-      <c r="G11" s="9">
-        <v>8.6347544528965692</v>
-      </c>
-      <c r="H11">
-        <v>4.64960051236356</v>
-      </c>
-      <c r="I11">
-        <v>21.850241129054901</v>
+        <v>34.770810258075699</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>10000</v>
       </c>
       <c r="J11" s="2">
         <v>10000</v>
@@ -999,156 +1010,156 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D12">
-        <v>34.8264118509572</v>
+        <v>6.6915635340299504</v>
       </c>
       <c r="E12">
-        <v>34.770810258075699</v>
-      </c>
-      <c r="F12" s="2">
-        <v>10000</v>
-      </c>
-      <c r="G12" s="10">
-        <v>10000</v>
-      </c>
-      <c r="H12" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I12" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J12" s="2">
-        <v>10000</v>
+        <v>14.275501381012701</v>
+      </c>
+      <c r="F12">
+        <v>32.074778430000002</v>
+      </c>
+      <c r="G12" s="9">
+        <v>31.074778429999999</v>
+      </c>
+      <c r="H12">
+        <v>32.132605853225002</v>
+      </c>
+      <c r="I12">
+        <v>4.64960051236356</v>
+      </c>
+      <c r="J12" s="8">
+        <v>21.489894238304199</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D13">
-        <v>6.6915635340299504</v>
+        <v>3.82375059232049</v>
       </c>
       <c r="E13">
-        <v>14.275501381012701</v>
+        <v>8.1574293605787105</v>
       </c>
       <c r="F13">
-        <v>32.074778430000002</v>
+        <v>18.328444815241401</v>
       </c>
       <c r="G13" s="9">
-        <v>31.074778429999999</v>
+        <v>16.328444815241401</v>
       </c>
       <c r="H13">
+        <v>18.361489058664102</v>
+      </c>
+      <c r="I13">
         <v>32.132605853225002</v>
       </c>
-      <c r="I13">
-        <v>4.64960051236356</v>
-      </c>
       <c r="J13" s="8">
-        <v>21.489894238304199</v>
+        <v>37.1533034709581</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>6</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D14">
-        <v>3.82375059232049</v>
+        <v>2.8075537209682202</v>
       </c>
       <c r="E14">
-        <v>8.1574293605787105</v>
+        <v>5.3040734518566</v>
       </c>
       <c r="F14">
-        <v>18.328444815241401</v>
+        <v>17.9353462175823</v>
       </c>
       <c r="G14" s="9">
-        <v>16.328444815241401</v>
+        <v>15.9353462175823</v>
       </c>
       <c r="H14">
-        <v>18.361489058664102</v>
+        <v>0.89330685185616898</v>
       </c>
       <c r="I14">
-        <v>32.132605853225002</v>
+        <v>9.7102422375552599</v>
       </c>
       <c r="J14" s="8">
-        <v>37.1533034709581</v>
+        <v>4.64960051236356</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>28</v>
       </c>
       <c r="D15">
-        <v>2.8075537209682202</v>
+        <v>8.0726718928761105</v>
       </c>
       <c r="E15">
-        <v>5.3040734518566</v>
+        <v>8.2395379153203194</v>
       </c>
       <c r="F15">
-        <v>17.9353462175823</v>
+        <v>42.426406845307298</v>
       </c>
       <c r="G15" s="9">
-        <v>15.9353462175823</v>
-      </c>
-      <c r="H15">
-        <v>0.89330685185616898</v>
-      </c>
-      <c r="I15">
-        <v>9.7102422375552599</v>
-      </c>
-      <c r="J15" s="8">
-        <v>4.64960051236356</v>
+        <v>11.4264068453073</v>
+      </c>
+      <c r="H15" s="23">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J15" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D16">
-        <v>8.0726718928761105</v>
+        <v>6.7419098980694496</v>
       </c>
       <c r="E16">
-        <v>8.2395379153203194</v>
+        <v>14.2287562812994</v>
       </c>
       <c r="F16">
-        <v>42.426406845307298</v>
+        <v>30.780288789055199</v>
       </c>
       <c r="G16" s="9">
-        <v>11.4264068453073</v>
-      </c>
-      <c r="H16" s="2">
-        <v>10000</v>
+        <v>27.780288789055199</v>
+      </c>
+      <c r="H16">
+        <v>30.855695875291399</v>
       </c>
       <c r="I16" s="2">
         <v>10000</v>
@@ -1159,95 +1170,95 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17">
-        <v>6.7419098980694496</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>14.2287562812994</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>30.780288789055199</v>
+        <v>0</v>
       </c>
       <c r="G17" s="9">
-        <v>27.780288789055199</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>30.855695875291399</v>
-      </c>
-      <c r="I17" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J17" s="2">
-        <v>10000</v>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>18.361489058664102</v>
+      </c>
+      <c r="J17" s="8">
+        <v>17.0996482487765</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>8.6927651945760296</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>10.8651495174042</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>9.6185105660554093</v>
       </c>
       <c r="G18" s="9">
-        <v>0</v>
+        <v>9.1185105660554093</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>9.7102422375552599</v>
       </c>
       <c r="I18">
-        <v>18.361489058664102</v>
-      </c>
-      <c r="J18" s="8">
-        <v>17.0996482487765</v>
+        <v>8.2592592273264902</v>
+      </c>
+      <c r="J18" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19">
         <v>10</v>
       </c>
       <c r="C19">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D19">
-        <v>8.6927651945760296</v>
+        <v>7.5088434251551597</v>
       </c>
       <c r="E19">
-        <v>10.8651495174042</v>
+        <v>8.8160519473920793</v>
       </c>
       <c r="F19">
-        <v>9.6185105660554093</v>
+        <v>10.806468350198401</v>
       </c>
       <c r="G19" s="9">
-        <v>9.1185105660554093</v>
+        <v>9.8064683501984007</v>
       </c>
       <c r="H19">
-        <v>9.7102422375552599</v>
+        <v>10.8402673609266</v>
       </c>
       <c r="I19">
-        <v>8.2592592273264902</v>
+        <v>1.8602452002122001</v>
       </c>
       <c r="J19" s="2">
         <v>10000</v>
@@ -1255,31 +1266,31 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D20">
-        <v>7.5088434251551597</v>
+        <v>11.8789282433822</v>
       </c>
       <c r="E20">
-        <v>8.8160519473920793</v>
+        <v>21.085862374984799</v>
       </c>
       <c r="F20">
-        <v>10.806468350198401</v>
+        <v>21.145112445761502</v>
       </c>
       <c r="G20" s="9">
-        <v>9.8064683501984007</v>
+        <v>20.945112445761499</v>
       </c>
       <c r="H20">
+        <v>21.134184835625899</v>
+      </c>
+      <c r="I20">
         <v>10.8402673609266</v>
-      </c>
-      <c r="I20">
-        <v>1.8602452002122001</v>
       </c>
       <c r="J20" s="2">
         <v>10000</v>
@@ -1287,31 +1298,31 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
       <c r="C21">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21">
-        <v>11.8789282433822</v>
-      </c>
-      <c r="E21">
-        <v>21.085862374984799</v>
-      </c>
-      <c r="F21">
-        <v>21.145112445761502</v>
-      </c>
-      <c r="G21" s="9">
-        <v>20.945112445761499</v>
-      </c>
-      <c r="H21">
-        <v>21.134184835625899</v>
-      </c>
-      <c r="I21">
-        <v>10.8402673609266</v>
+        <v>9.2765811457867908</v>
+      </c>
+      <c r="E21" s="3">
+        <v>27.644193735440702</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H21" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="2">
+        <v>10000</v>
       </c>
       <c r="J21" s="2">
         <v>10000</v>
@@ -1319,19 +1330,19 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C22">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D22">
-        <v>9.2765811457867908</v>
-      </c>
-      <c r="E22" s="3">
-        <v>27.644193735440702</v>
+        <v>38.140142472224099</v>
+      </c>
+      <c r="E22" s="2">
+        <v>10000</v>
       </c>
       <c r="F22" s="2">
         <v>10000</v>
@@ -1351,31 +1362,31 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>12</v>
       </c>
       <c r="C23">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D23">
-        <v>38.140142472224099</v>
-      </c>
-      <c r="E23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="G23" s="10">
-        <v>10000</v>
-      </c>
-      <c r="H23" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I23" s="2">
-        <v>10000</v>
+        <v>5.4590196573633198</v>
+      </c>
+      <c r="E23">
+        <v>3.4202295674286201</v>
+      </c>
+      <c r="F23">
+        <v>6.8613315699296198</v>
+      </c>
+      <c r="G23" s="9">
+        <v>7.2161331569929601</v>
+      </c>
+      <c r="H23">
+        <v>6.8450956589299601</v>
+      </c>
+      <c r="I23">
+        <v>30.855695875291399</v>
       </c>
       <c r="J23" s="2">
         <v>10000</v>
@@ -1383,31 +1394,31 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24">
         <v>12</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D24">
-        <v>5.4590196573633198</v>
+        <v>9.5365035274049905</v>
       </c>
       <c r="E24">
-        <v>3.4202295674286201</v>
+        <v>5.7047657163407202</v>
       </c>
       <c r="F24">
-        <v>6.8613315699296198</v>
+        <v>13.7316983454739</v>
       </c>
       <c r="G24" s="9">
-        <v>7.2161331569929601</v>
+        <v>13.521698345324699</v>
       </c>
       <c r="H24">
-        <v>6.8450956589299601</v>
+        <v>13.6944519707334</v>
       </c>
       <c r="I24">
-        <v>30.855695875291399</v>
+        <v>41.058257494958397</v>
       </c>
       <c r="J24" s="2">
         <v>10000</v>
@@ -1415,31 +1426,31 @@
     </row>
     <row r="25" spans="1:10">
       <c r="A25">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>12</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25">
-        <v>9.5365035274049905</v>
+        <v>9.2641818094680897</v>
       </c>
       <c r="E25">
-        <v>5.7047657163407202</v>
+        <v>3.9221165420248498</v>
       </c>
       <c r="F25">
-        <v>13.7316983454739</v>
+        <v>5.1888727825468104</v>
       </c>
       <c r="G25" s="9">
-        <v>13.521698345324699</v>
+        <v>6.2688727825468096</v>
       </c>
       <c r="H25">
-        <v>13.6944519707334</v>
+        <v>5.0663957899459602</v>
       </c>
       <c r="I25">
-        <v>41.058257494958397</v>
+        <v>6.8450956589299601</v>
       </c>
       <c r="J25" s="2">
         <v>10000</v>
@@ -1447,31 +1458,31 @@
     </row>
     <row r="26" spans="1:10">
       <c r="A26">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D26">
-        <v>9.2641818094680897</v>
+        <v>1.16706216891694</v>
       </c>
       <c r="E26">
-        <v>3.9221165420248498</v>
+        <v>3.2034666516399701</v>
       </c>
       <c r="F26">
-        <v>5.1888727825468104</v>
+        <v>0.482175305837025</v>
       </c>
       <c r="G26" s="9">
-        <v>6.2688727825468096</v>
+        <v>0.74217530583702496</v>
       </c>
       <c r="H26">
-        <v>5.0663957899459602</v>
+        <v>0.45133919580828402</v>
       </c>
       <c r="I26">
-        <v>6.8450956589299601</v>
+        <v>13.6944519707334</v>
       </c>
       <c r="J26" s="2">
         <v>10000</v>
@@ -1479,31 +1490,31 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D27">
-        <v>1.16706216891694</v>
+        <v>9.1960278750704703</v>
       </c>
       <c r="E27">
-        <v>3.2034666516399701</v>
+        <v>7.2461322124278098</v>
       </c>
       <c r="F27">
-        <v>0.482175305837025</v>
+        <v>5.2707429949098401</v>
       </c>
       <c r="G27" s="9">
-        <v>0.74217530583702496</v>
+        <v>8.2707429949098401</v>
       </c>
       <c r="H27">
+        <v>5.2196286993339802</v>
+      </c>
+      <c r="I27">
         <v>0.45133919580828402</v>
-      </c>
-      <c r="I27">
-        <v>13.6944519707334</v>
       </c>
       <c r="J27" s="2">
         <v>10000</v>
@@ -1511,31 +1522,31 @@
     </row>
     <row r="28" spans="1:10">
       <c r="A28">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>15</v>
       </c>
       <c r="C28">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D28">
-        <v>9.1960278750704703</v>
+        <v>10.250814838659201</v>
       </c>
       <c r="E28">
-        <v>7.2461322124278098</v>
-      </c>
-      <c r="F28">
-        <v>5.2707429949098401</v>
-      </c>
-      <c r="G28" s="9">
-        <v>8.2707429949098401</v>
-      </c>
-      <c r="H28">
-        <v>5.2196286993339802</v>
-      </c>
-      <c r="I28">
-        <v>0.45133919580828402</v>
+        <v>19.634976234570601</v>
+      </c>
+      <c r="F28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G28" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I28" s="2">
+        <v>10000</v>
       </c>
       <c r="J28" s="2">
         <v>10000</v>
@@ -1543,31 +1554,31 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D29">
-        <v>10.250814838659201</v>
+        <v>6.05193214017884</v>
       </c>
       <c r="E29">
-        <v>19.634976234570601</v>
-      </c>
-      <c r="F29" s="2">
-        <v>10000</v>
-      </c>
-      <c r="G29" s="10">
-        <v>10000</v>
-      </c>
-      <c r="H29" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I29" s="2">
-        <v>10000</v>
+        <v>0.206143663213262</v>
+      </c>
+      <c r="F29">
+        <v>1.38493599653073</v>
+      </c>
+      <c r="G29" s="9">
+        <v>1.913599653073</v>
+      </c>
+      <c r="H29">
+        <v>1.1794811247678501</v>
+      </c>
+      <c r="I29">
+        <v>5.0663957899459602</v>
       </c>
       <c r="J29" s="2">
         <v>10000</v>
@@ -1575,31 +1586,31 @@
     </row>
     <row r="30" spans="1:10">
       <c r="A30">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C30">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D30">
-        <v>6.05193214017884</v>
+        <v>5.8772751729399397</v>
       </c>
       <c r="E30">
-        <v>0.206143663213262</v>
+        <v>3.8909925651811701</v>
       </c>
       <c r="F30">
-        <v>1.38493599653073</v>
+        <v>1.9317436821802301</v>
       </c>
       <c r="G30" s="9">
-        <v>1.913599653073</v>
+        <v>4.6317436821802298</v>
       </c>
       <c r="H30">
+        <v>1.8602452002122001</v>
+      </c>
+      <c r="I30">
         <v>1.1794811247678501</v>
-      </c>
-      <c r="I30">
-        <v>5.0663957899459602</v>
       </c>
       <c r="J30" s="2">
         <v>10000</v>
@@ -1607,31 +1618,31 @@
     </row>
     <row r="31" spans="1:10">
       <c r="A31">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31">
-        <v>5.8772751729399397</v>
+        <v>5.2589125824513898</v>
       </c>
       <c r="E31">
-        <v>3.8909925651811701</v>
+        <v>6.37667245979911</v>
       </c>
       <c r="F31">
-        <v>1.9317436821802301</v>
+        <v>8.2241179959573198</v>
       </c>
       <c r="G31" s="9">
-        <v>4.6317436821802298</v>
+        <v>9.2241179959573198</v>
       </c>
       <c r="H31">
-        <v>1.8602452002122001</v>
+        <v>8.2592592273264902</v>
       </c>
       <c r="I31">
-        <v>1.1794811247678501</v>
+        <v>5.2196286993339802</v>
       </c>
       <c r="J31" s="2">
         <v>10000</v>
@@ -1639,31 +1650,31 @@
     </row>
     <row r="32" spans="1:10">
       <c r="A32">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D32">
-        <v>5.2589125824513898</v>
-      </c>
-      <c r="E32">
-        <v>6.37667245979911</v>
-      </c>
-      <c r="F32">
-        <v>8.2241179959573198</v>
-      </c>
-      <c r="G32" s="9">
-        <v>9.2241179959573198</v>
-      </c>
-      <c r="H32">
-        <v>8.2592592273264902</v>
-      </c>
-      <c r="I32">
-        <v>5.2196286993339802</v>
+        <v>30.310424669747999</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F32" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G32" s="10">
+        <v>10000</v>
+      </c>
+      <c r="H32" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I32" s="2">
+        <v>10000</v>
       </c>
       <c r="J32" s="2">
         <v>10000</v>
@@ -1671,330 +1682,321 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D33">
-        <v>30.310424669747999</v>
-      </c>
-      <c r="E33" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F33" s="2">
-        <v>10000</v>
-      </c>
-      <c r="G33" s="10">
-        <v>10000</v>
-      </c>
-      <c r="H33" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I33" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J33" s="2">
-        <v>10000</v>
+        <v>8.0760670620418402</v>
+      </c>
+      <c r="E33">
+        <v>5.7971639394608596</v>
+      </c>
+      <c r="F33">
+        <v>22.020682171325301</v>
+      </c>
+      <c r="G33" s="9">
+        <v>12.0206821713253</v>
+      </c>
+      <c r="H33">
+        <v>12.7807246021501</v>
+      </c>
+      <c r="I33">
+        <v>12.7807246021501</v>
+      </c>
+      <c r="J33" s="6">
+        <v>12.7807246021501</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>24</v>
       </c>
       <c r="D34">
-        <v>8.0760670620418402</v>
+        <v>7.1402444938851799</v>
       </c>
       <c r="E34">
-        <v>5.7971639394608596</v>
+        <v>4.4038015386183904</v>
       </c>
       <c r="F34">
-        <v>22.020682171325301</v>
+        <v>16.0306170602151</v>
       </c>
       <c r="G34" s="9">
-        <v>12.0206821713253</v>
+        <v>13.976306170602101</v>
       </c>
       <c r="H34">
-        <v>12.7807246021501</v>
+        <v>16.3118816827008</v>
       </c>
       <c r="I34">
-        <v>12.7807246021501</v>
+        <v>16.3118816827008</v>
       </c>
       <c r="J34" s="6">
-        <v>12.7807246021501</v>
+        <v>16.3118816827008</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C35">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D35">
-        <v>7.1402444938851799</v>
+        <v>4.2421987525588296</v>
       </c>
       <c r="E35">
-        <v>4.4038015386183904</v>
+        <v>6.7254394020000001</v>
       </c>
       <c r="F35">
-        <v>16.0306170602151</v>
+        <v>31.083896135674699</v>
       </c>
       <c r="G35" s="9">
-        <v>13.976306170602101</v>
-      </c>
-      <c r="H35">
-        <v>16.3118816827008</v>
-      </c>
-      <c r="I35">
-        <v>16.3118816827008</v>
-      </c>
-      <c r="J35" s="6">
-        <v>16.3118816827008</v>
+        <v>11.083896135674699</v>
+      </c>
+      <c r="H35" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I35" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J35" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C36">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D36">
-        <v>4.2421987525588296</v>
+        <v>4.2657089528143803</v>
       </c>
       <c r="E36">
-        <v>6.7254394020000001</v>
+        <v>4.2657658525350097</v>
       </c>
       <c r="F36">
-        <v>31.083896135674699</v>
+        <v>4.2671188565547702</v>
       </c>
       <c r="G36" s="9">
-        <v>11.083896135674699</v>
-      </c>
-      <c r="H36" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I36" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J36" s="2">
-        <v>10000</v>
+        <v>7.2671188565547702</v>
+      </c>
+      <c r="H36">
+        <v>4.2655764313671698</v>
+      </c>
+      <c r="I36">
+        <v>4.2655764313671698</v>
+      </c>
+      <c r="J36" s="5">
+        <v>4.2655764313671698</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>25</v>
       </c>
       <c r="C37">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D37">
-        <v>4.2657089528143803</v>
+        <v>7.4677896238322701</v>
       </c>
       <c r="E37">
-        <v>4.2657658525350097</v>
+        <v>9.6982785011312203</v>
       </c>
       <c r="F37">
-        <v>4.2671188565547702</v>
+        <v>29.6146112387272</v>
       </c>
       <c r="G37" s="9">
-        <v>7.2671188565547702</v>
+        <v>9.6146112387271998</v>
       </c>
       <c r="H37">
-        <v>4.2655764313671698</v>
+        <v>4.2655764313815201</v>
       </c>
       <c r="I37">
-        <v>4.2655764313671698</v>
+        <v>4.2655764313815201</v>
       </c>
       <c r="J37" s="5">
-        <v>4.2655764313671698</v>
+        <v>4.2655764313815201</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B38">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C38">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D38">
-        <v>7.4677896238322701</v>
+        <v>6.3994350255268904</v>
       </c>
       <c r="E38">
-        <v>9.6982785011312203</v>
+        <v>6.3994350271494502</v>
       </c>
       <c r="F38">
-        <v>29.6146112387272</v>
+        <v>6.39943502714942</v>
       </c>
       <c r="G38" s="9">
-        <v>9.6146112387271998</v>
+        <v>8.3994350271494191</v>
       </c>
       <c r="H38">
-        <v>4.2655764313815201</v>
+        <v>6.3994350255268904</v>
       </c>
       <c r="I38">
-        <v>4.2655764313815201</v>
+        <v>6.3994350255268904</v>
       </c>
       <c r="J38" s="5">
-        <v>4.2655764313815201</v>
+        <v>6.3994350255268904</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B39">
         <v>27</v>
       </c>
       <c r="C39">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D39">
-        <v>6.3994350255268904</v>
+        <v>7.31660240824338</v>
       </c>
       <c r="E39">
-        <v>6.3994350271494502</v>
+        <v>7.3166024113780601</v>
       </c>
       <c r="F39">
-        <v>6.39943502714942</v>
+        <v>7.3166024113780601</v>
       </c>
       <c r="G39" s="9">
-        <v>8.3994350271494191</v>
+        <v>9.3166024113780601</v>
       </c>
       <c r="H39">
-        <v>6.3994350255268904</v>
+        <v>7.3166024082433703</v>
       </c>
       <c r="I39">
-        <v>6.3994350255268904</v>
+        <v>7.3166024082433703</v>
       </c>
       <c r="J39" s="5">
-        <v>6.3994350255268904</v>
+        <v>7.3166024082433703</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40">
+        <v>28</v>
+      </c>
+      <c r="C40">
         <v>27</v>
       </c>
-      <c r="C40">
-        <v>30</v>
-      </c>
       <c r="D40">
-        <v>7.31660240824338</v>
+        <v>8.6251332572782502</v>
       </c>
       <c r="E40">
-        <v>7.3166024113780601</v>
+        <v>10.0289950170414</v>
       </c>
       <c r="F40">
-        <v>7.3166024113780601</v>
+        <v>38.362653135260103</v>
       </c>
       <c r="G40" s="9">
-        <v>9.3166024113780601</v>
-      </c>
-      <c r="H40">
-        <v>7.3166024082433703</v>
-      </c>
-      <c r="I40">
-        <v>7.3166024082433703</v>
-      </c>
-      <c r="J40" s="5">
-        <v>7.3166024082433703</v>
+        <v>8.3626531352600999</v>
+      </c>
+      <c r="H40" s="23">
+        <v>10000</v>
+      </c>
+      <c r="I40" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J40" s="2">
+        <v>10000</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B41">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C41">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D41">
-        <v>8.6251332572782502</v>
+        <v>3.7342810122603698</v>
       </c>
       <c r="E41">
-        <v>10.0289950170414</v>
+        <v>3.73428101489263</v>
       </c>
       <c r="F41">
-        <v>38.362653135260103</v>
+        <v>3.73428101489265</v>
       </c>
       <c r="G41" s="9">
-        <v>8.3626531352600999</v>
-      </c>
-      <c r="H41" s="2">
-        <v>10000</v>
-      </c>
-      <c r="I41" s="2">
-        <v>10000</v>
-      </c>
-      <c r="J41" s="2">
-        <v>10000</v>
+        <v>7.73428101489265</v>
+      </c>
+      <c r="H41">
+        <v>3.7342810122603698</v>
+      </c>
+      <c r="I41">
+        <v>3.7342810122603698</v>
+      </c>
+      <c r="J41" s="5">
+        <v>3.7342810122603698</v>
       </c>
     </row>
     <row r="42" spans="1:10">
-      <c r="A42">
-        <v>39</v>
-      </c>
-      <c r="B42">
-        <v>29</v>
-      </c>
-      <c r="C42">
-        <v>30</v>
-      </c>
-      <c r="D42">
-        <v>3.7342810122603698</v>
-      </c>
-      <c r="E42">
-        <v>3.73428101489263</v>
-      </c>
-      <c r="F42">
-        <v>3.73428101489265</v>
-      </c>
-      <c r="G42" s="9">
-        <v>7.73428101489265</v>
-      </c>
-      <c r="H42">
-        <v>3.7342810122603698</v>
-      </c>
-      <c r="I42">
-        <v>3.7342810122603698</v>
-      </c>
-      <c r="J42" s="5">
-        <v>3.7342810122603698</v>
+      <c r="B42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:10">
-      <c r="B43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>1</v>
+      <c r="D43" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" t="s">
+        <v>9</v>
+      </c>
+      <c r="J43" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="14.25" thickBot="1"/>
@@ -2150,9 +2152,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:J64">
-    <sortCondition ref="B1:B64"/>
-    <sortCondition ref="C1:C64"/>
+  <sortState ref="A1:J58">
+    <sortCondition ref="B1:B58"/>
+    <sortCondition ref="C1:C58"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2164,7 +2166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD21"/>
     </sheetView>
   </sheetViews>

</xml_diff>